<commit_message>
set columns format to the whole sheet
</commit_message>
<xml_diff>
--- a/tests/data/cols/foreignkey.xlsx
+++ b/tests/data/cols/foreignkey.xlsx
@@ -61,8 +61,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode=""/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##"/>
+    <numFmt numFmtId="165" formatCode=""/>
+    <numFmt numFmtId="165" formatCode=""/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -101,9 +103,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -405,12 +413,16 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
handle required and set protection
</commit_message>
<xml_diff>
--- a/tests/data/cols/foreignkey.xlsx
+++ b/tests/data/cols/foreignkey.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>null</t>
   </si>
@@ -50,7 +50,16 @@
     <t>Id</t>
   </si>
   <si>
+    <t>AutoColumn</t>
+  </si>
+  <si>
     <t>Option</t>
+  </si>
+  <si>
+    <t>ForeignKeyColumn</t>
+  </si>
+  <si>
+    <t>number,unique,min,max</t>
   </si>
   <si>
     <t>Option 0</t>
@@ -148,7 +157,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -464,11 +475,11 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection objects="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="2">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a value between -2147483648 and 2147483647&#10;No duplicates allowed in this column" sqref="A2:A65001">
       <formula1>AND(ISNUMBER(VALUE(THIS)),COUNTIF(INDIRECT(ADDRESS(1,COLUMN()) &amp; ":" &amp; ADDRESS(65536, COLUMN())),THIS)=1,VALUE(THIS)&gt;=-2147483648,VALUE(THIS)&lt;=2147483647)</formula1>
@@ -483,7 +494,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -494,7 +505,7 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -565,6 +576,19 @@
       </c>
       <c r="C9" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -593,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -601,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -609,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -617,7 +641,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -625,7 +649,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -633,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -641,7 +665,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -649,7 +673,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -657,11 +681,11 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection objects="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>